<commit_message>
Correct typo in URI for quarterly frequency.
</commit_message>
<xml_diff>
--- a/spec/ConvSpec-006-008-v1.5.xlsx
+++ b/spec/ConvSpec-006-008-v1.5.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="1176">
   <si>
     <t>ignore</t>
   </si>
@@ -2999,9 +2999,6 @@
     <t>## - http://id.loc.gov/vocabulary/frequencies/mon</t>
   </si>
   <si>
-    <t>## - http://id.loc.gov/vocabulary/frequencies/grt</t>
-  </si>
-  <si>
     <t>## - http://id.loc.gov/vocabulary/frequencies/smn</t>
   </si>
   <si>
@@ -3599,7 +3596,13 @@
     <t>W - supplementaryContent - SupplementaryContent - http://id.loc.gov/vocabulary/msupplcont/index</t>
   </si>
   <si>
-    <t>Fields 006, 008 - Fixed general and additional - v1.5, 05/20/2019</t>
+    <t>1.6 -- change to supplementary content vocab?</t>
+  </si>
+  <si>
+    <t>## - http://id.loc.gov/vocabulary/frequencies/qrt</t>
+  </si>
+  <si>
+    <t>Fields 006, 008 - Fixed general and additional - v1.5, 06/03/2019</t>
   </si>
 </sst>
 </file>
@@ -3656,7 +3659,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3666,12 +3669,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3704,7 +3701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3740,9 +3737,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4026,10 +4020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D581"/>
+  <dimension ref="A1:F581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C490" sqref="C490"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4046,7 +4040,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>513</v>
@@ -4060,7 +4054,7 @@
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>577</v>
@@ -4513,7 +4507,7 @@
         <v>102</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4809,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>129</v>
       </c>
@@ -4817,7 +4811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>130</v>
       </c>
@@ -4825,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>131</v>
       </c>
@@ -4836,7 +4830,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>132</v>
       </c>
@@ -4847,7 +4841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>133</v>
       </c>
@@ -4858,29 +4852,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B103" s="5" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>1108</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>136</v>
       </c>
@@ -4891,40 +4885,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>46</v>
       </c>
@@ -4932,15 +4926,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B109" s="13" t="s">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="9" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>141</v>
       </c>
@@ -4948,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>142</v>
       </c>
@@ -4958,8 +4952,11 @@
       <c r="C111" s="6" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F111" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>143</v>
       </c>
@@ -5480,7 +5477,7 @@
         <v>188</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C163" s="5" t="s">
         <v>955</v>
@@ -5754,10 +5751,10 @@
         <v>137</v>
       </c>
       <c r="B193" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C193" s="5" t="s">
         <v>1166</v>
-      </c>
-      <c r="C193" s="5" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -5855,7 +5852,7 @@
         <v>219</v>
       </c>
       <c r="B203" s="10" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>33</v>
@@ -5946,7 +5943,7 @@
         <v>225</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -5962,10 +5959,10 @@
         <v>227</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -5973,10 +5970,10 @@
         <v>228</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -5984,10 +5981,10 @@
         <v>229</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -5995,10 +5992,10 @@
         <v>230</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6006,10 +6003,10 @@
         <v>231</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6017,10 +6014,10 @@
         <v>232</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6028,10 +6025,10 @@
         <v>233</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6039,10 +6036,10 @@
         <v>234</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6050,10 +6047,10 @@
         <v>235</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6061,10 +6058,10 @@
         <v>236</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6072,10 +6069,10 @@
         <v>237</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -6099,7 +6096,7 @@
         <v>239</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -6115,10 +6112,10 @@
         <v>241</v>
       </c>
       <c r="B232" s="5" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C232" s="5" t="s">
         <v>1007</v>
-      </c>
-      <c r="C232" s="5" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6126,10 +6123,10 @@
         <v>242</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6137,10 +6134,10 @@
         <v>243</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6148,10 +6145,10 @@
         <v>244</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6159,10 +6156,10 @@
         <v>245</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C236" s="5" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6170,10 +6167,10 @@
         <v>246</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6181,10 +6178,10 @@
         <v>247</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6192,10 +6189,10 @@
         <v>248</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6203,10 +6200,10 @@
         <v>249</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6214,10 +6211,10 @@
         <v>250</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6225,10 +6222,10 @@
         <v>251</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6236,10 +6233,10 @@
         <v>252</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6247,10 +6244,10 @@
         <v>253</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6258,10 +6255,10 @@
         <v>254</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6269,10 +6266,10 @@
         <v>255</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6280,10 +6277,10 @@
         <v>256</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6291,10 +6288,10 @@
         <v>257</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C248" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6302,10 +6299,10 @@
         <v>258</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="250" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6313,10 +6310,10 @@
         <v>259</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6324,10 +6321,10 @@
         <v>260</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C251" s="5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6335,10 +6332,10 @@
         <v>261</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C252" s="5" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6346,10 +6343,10 @@
         <v>262</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C253" s="5" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6357,10 +6354,10 @@
         <v>263</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6368,10 +6365,10 @@
         <v>264</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C255" s="5" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6379,10 +6376,10 @@
         <v>265</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C256" s="5" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6390,10 +6387,10 @@
         <v>266</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C257" s="5" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6401,10 +6398,10 @@
         <v>267</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6412,10 +6409,10 @@
         <v>268</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6423,10 +6420,10 @@
         <v>269</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6434,10 +6431,10 @@
         <v>270</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6445,10 +6442,10 @@
         <v>271</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6456,10 +6453,10 @@
         <v>272</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="264" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6467,10 +6464,10 @@
         <v>273</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6478,10 +6475,10 @@
         <v>274</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6489,10 +6486,10 @@
         <v>275</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6500,10 +6497,10 @@
         <v>276</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C267" s="5" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="268" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6511,10 +6508,10 @@
         <v>277</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C268" s="5" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6522,10 +6519,10 @@
         <v>278</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C269" s="5" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6533,10 +6530,10 @@
         <v>279</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C270" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="271" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -6544,10 +6541,10 @@
         <v>280</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -6555,10 +6552,10 @@
         <v>281</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -6566,10 +6563,10 @@
         <v>282</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -6577,10 +6574,10 @@
         <v>283</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C274" s="5" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -6588,10 +6585,10 @@
         <v>284</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -6599,10 +6596,10 @@
         <v>285</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C276" s="5" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -6634,7 +6631,7 @@
         <v>287</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C280" s="5"/>
     </row>
@@ -6643,10 +6640,10 @@
         <v>288</v>
       </c>
       <c r="B281" s="12" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -6654,10 +6651,10 @@
         <v>289</v>
       </c>
       <c r="B282" s="12" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -6665,10 +6662,10 @@
         <v>290</v>
       </c>
       <c r="B283" s="12" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -6676,7 +6673,7 @@
         <v>51</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C284" s="6" t="s">
         <v>735</v>
@@ -6687,7 +6684,7 @@
         <v>291</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C285" s="6" t="s">
         <v>736</v>
@@ -7970,7 +7967,7 @@
         <v>398</v>
       </c>
       <c r="B416" s="5" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
@@ -7986,10 +7983,10 @@
         <v>400</v>
       </c>
       <c r="B418" s="5" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C418" s="5" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -7997,10 +7994,10 @@
         <v>401</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C419" s="5" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8008,10 +8005,10 @@
         <v>402</v>
       </c>
       <c r="B420" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C420" s="5" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="421" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -8019,10 +8016,10 @@
         <v>403</v>
       </c>
       <c r="B421" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C421" s="5" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8030,10 +8027,10 @@
         <v>404</v>
       </c>
       <c r="B422" s="5" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C422" s="5" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8041,10 +8038,10 @@
         <v>405</v>
       </c>
       <c r="B423" s="5" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C423" s="5" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="63" x14ac:dyDescent="0.25">
@@ -8052,10 +8049,10 @@
         <v>406</v>
       </c>
       <c r="B424" s="5" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C424" s="5" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8063,10 +8060,10 @@
         <v>407</v>
       </c>
       <c r="B425" s="5" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C425" s="5" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8074,10 +8071,10 @@
         <v>408</v>
       </c>
       <c r="B426" s="5" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C426" s="5" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8085,10 +8082,10 @@
         <v>409</v>
       </c>
       <c r="B427" s="5" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C427" s="5" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
@@ -8096,10 +8093,10 @@
         <v>410</v>
       </c>
       <c r="B428" s="5" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C428" s="5" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -8107,7 +8104,7 @@
         <v>411</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>638</v>
@@ -8578,7 +8575,7 @@
         <v>450</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>1174</v>
       </c>
       <c r="C481" s="6" t="s">
         <v>913</v>
@@ -8589,7 +8586,7 @@
         <v>451</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C482" s="6" t="s">
         <v>914</v>
@@ -8600,7 +8597,7 @@
         <v>452</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C483" s="6" t="s">
         <v>915</v>
@@ -8620,7 +8617,7 @@
         <v>453</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C485" s="6" t="s">
         <v>916</v>
@@ -8647,7 +8644,7 @@
         <v>454</v>
       </c>
       <c r="B488" s="9" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C488" s="5"/>
     </row>
@@ -8656,10 +8653,10 @@
         <v>455</v>
       </c>
       <c r="B489" s="9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C489" s="5" t="s">
         <v>1135</v>
-      </c>
-      <c r="C489" s="5" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.25">
@@ -8685,10 +8682,10 @@
         <v>457</v>
       </c>
       <c r="B492" s="9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C492" s="5" t="s">
         <v>1135</v>
-      </c>
-      <c r="C492" s="5" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.25">
@@ -8855,7 +8852,7 @@
         <v>470</v>
       </c>
       <c r="B511" s="5" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C511" s="5"/>
     </row>
@@ -8873,10 +8870,10 @@
         <v>472</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C513" s="5" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="514" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -8884,10 +8881,10 @@
         <v>473</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C514" s="5" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.25">
@@ -8895,10 +8892,10 @@
         <v>474</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C515" s="5" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
@@ -8906,10 +8903,10 @@
         <v>475</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C516" s="5" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.25">
@@ -8917,10 +8914,10 @@
         <v>476</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C517" s="5" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.25">
@@ -8928,10 +8925,10 @@
         <v>477</v>
       </c>
       <c r="B518" s="5" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C518" s="5" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
@@ -8939,10 +8936,10 @@
         <v>478</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C519" s="5" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.25">
@@ -8950,10 +8947,10 @@
         <v>479</v>
       </c>
       <c r="B520" s="5" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C520" s="5" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
@@ -8961,10 +8958,10 @@
         <v>480</v>
       </c>
       <c r="B521" s="5" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C521" s="5" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
@@ -8972,10 +8969,10 @@
         <v>481</v>
       </c>
       <c r="B522" s="5" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C522" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.25">
@@ -8983,10 +8980,10 @@
         <v>482</v>
       </c>
       <c r="B523" s="5" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C523" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.25">
@@ -8994,10 +8991,10 @@
         <v>483</v>
       </c>
       <c r="B524" s="5" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C524" s="5" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
@@ -9043,7 +9040,7 @@
         <v>556</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="530" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -9054,7 +9051,7 @@
         <v>557</v>
       </c>
       <c r="C530" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="531" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -9065,7 +9062,7 @@
         <v>555</v>
       </c>
       <c r="C531" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="532" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -9076,7 +9073,7 @@
         <v>0</v>
       </c>
       <c r="C532" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">
@@ -9427,7 +9424,7 @@
         <v>949</v>
       </c>
       <c r="D570" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="571" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -9441,7 +9438,7 @@
         <v>950</v>
       </c>
       <c r="D571" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.25">
@@ -9455,7 +9452,7 @@
         <v>951</v>
       </c>
       <c r="D572" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>